<commit_message>
creating random stations during import, using compound index, querying full timestamp ranges
</commit_message>
<xml_diff>
--- a/docs/results/Testbed_3/results_testbed3.xlsx
+++ b/docs/results/Testbed_3/results_testbed3.xlsx
@@ -11,7 +11,6 @@
     <sheet name="_ID SHARD KEY" sheetId="4" r:id="rId2"/>
     <sheet name="COMBINED SHARD KEY" sheetId="5" r:id="rId3"/>
     <sheet name="RESULTS" sheetId="3" r:id="rId4"/>
-    <sheet name="Tabelle1" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_30M" localSheetId="0">'TIMESTAMP SHARD KEY'!$A$1:$E$249</definedName>
@@ -914,24 +913,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="76484992"/>
-        <c:axId val="76486528"/>
+        <c:axId val="104292352"/>
+        <c:axId val="104293888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="76484992"/>
+        <c:axId val="104292352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76486528"/>
+        <c:crossAx val="104293888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76486528"/>
+        <c:axId val="104293888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -957,7 +956,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76484992"/>
+        <c:crossAx val="104292352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -970,7 +969,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6437,7 +6436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H249"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A153" sqref="A153"/>
     </sheetView>
   </sheetViews>
@@ -9001,7 +9000,7 @@
   <dimension ref="A2:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9176,16 +9175,4 @@
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>